<commit_message>
APP_VERSION; import working but needs import status kept and used from update_labels_field-import and generate_markers-import
</commit_message>
<xml_diff>
--- a/egdata/scatterplot.xlsx
+++ b/egdata/scatterplot.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jboucas/flaski-3.0.0/egdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89753501-E017-4D41-A94E-220A0E3E93AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6DC3F0-030A-134F-A938-8718EF4CD84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{6DBC6587-9E73-044F-93EA-3A9AA4279C24}"/>
   </bookViews>
@@ -32,12 +32,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>X</t>
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -389,60 +398,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD143A5F-6BBF-9346-A793-E1DC454ADC95}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>